<commit_message>
- remove file excel (not use)
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Download/kangjindemo/28fef5a1-f0f2-4b94-a4ad-081b227f3b77/BaoCaoNhatKyChiTien.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Download/kangjindemo/28fef5a1-f0f2-4b94-a4ad-081b227f3b77/BaoCaoNhatKyChiTien.xlsx
@@ -29,11 +29,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Tổng cộng:</t>
+  </si>
+  <si>
+    <t>BÁO CÁO NHẬT KÝ CHI TIỀN</t>
+  </si>
   <si>
     <t>Mã người nhận</t>
   </si>
   <si>
+    <t>Nhóm đối tác</t>
+  </si>
+  <si>
     <t>Hóa đơn liên quan</t>
   </si>
   <si>
@@ -61,6 +70,12 @@
     <t>Tiền mặt</t>
   </si>
   <si>
+    <t>Chuyển khoản</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
     <t>Số tài khoản</t>
   </si>
   <si>
@@ -68,6 +83,15 @@
   </si>
   <si>
     <t>Tiền chi</t>
+  </si>
+  <si>
+    <t>Từ ngày 29/08/2022 đến ngày 04/09/2022</t>
+  </si>
+  <si>
+    <t>Chi nhánh: KangjinDemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kangjin Sài Gòn CS2, </t>
   </si>
   <si>
     <t>TH0000000002</t>
@@ -161,7 +185,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799979984760284"/>
+        <fgColor theme="8" tint="0.79998"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +756,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -742,19 +766,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.75" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="25" customWidth="1"/>
-    <col min="4" max="4" width="16.375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="18.75" style="4" customWidth="1"/>
-    <col min="6" max="7" width="14.75" style="7" customWidth="1"/>
-    <col min="8" max="10" width="16.375" style="21" customWidth="1"/>
-    <col min="11" max="12" width="14.75" style="18" customWidth="1"/>
-    <col min="13" max="13" width="29.875" style="14" customWidth="1"/>
-    <col min="14" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="31.25" style="4" customWidth="1"/>
+    <col min="2" max="3" width="18.75" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16.375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="18.75" style="4" customWidth="1"/>
+    <col min="7" max="10" width="14.75" style="7" customWidth="1"/>
+    <col min="11" max="13" width="16.375" style="21" customWidth="1"/>
+    <col min="14" max="15" width="14.75" style="18" customWidth="1"/>
+    <col min="16" max="16" width="29.875" style="14" customWidth="1"/>
+    <col min="17" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="34.5" customHeight="1">
-      <c r="A1" s="29"/>
+    <row r="1" spans="1:17" ht="34.5" customHeight="1">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -767,10 +794,15 @@
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
-      <c r="N1" s="2"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="30"/>
+    <row r="2" spans="1:16" ht="15">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -783,112 +815,147 @@
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
       <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
-    <row r="3" ht="15">
-      <c r="A3" s="9"/>
+    <row r="3" spans="1:2" ht="15">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="14.25">
+    <row r="4" spans="1:16" s="5" customFormat="1" ht="14.25">
       <c r="A4" s="10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>9</v>
+      <c r="F4" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>5</v>
+      <c r="H4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>8</v>
       </c>
+      <c r="N4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="15">
+    <row r="5" spans="1:16" ht="15">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="27">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="27">
         <v>44802.5845833333</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="6">
-        <v>27020000</v>
+      <c r="E5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="G5" s="6">
         <v>27020000</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>19</v>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>27020000</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21.75" customHeight="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="8">
-        <f>SUM(F$5:F5)</f>
+    <row r="6" spans="1:16" ht="21.75" customHeight="1">
+      <c r="A6" s="31" t="s">
         <v>0</v>
       </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="8">
         <f>SUM(G$5:G5)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
+      <c r="H6" s="8">
+        <f>SUM(H$5:H5)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <f>SUM(I$5:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="8">
+        <f>SUM(J$5:J5)</f>
+        <v>0</v>
+      </c>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
-      <c r="M6" s="17"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup orientation="landscape" scale="95" r:id="rId1"/>

</xml_diff>